<commit_message>
Add bilingual tags and regenerate workbook
</commit_message>
<xml_diff>
--- a/image_descriptions.xlsx
+++ b/image_descriptions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,12 +446,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>description_en</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tag</t>
+          <t>description_th</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>tags_en</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>tags_th</t>
         </is>
       </c>
     </row>
@@ -468,12 +478,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>This charming star-shaped pendant features a smooth, glossy turquoise surface with subtle layered detailing. It is accented with a small gold ball at the base and a gold loop at the top, perfect for attaching to a necklace or bracelet. The design is playful yet elegant, ideal for everyday wear.</t>
+          <t>This product is a star-shaped pendant with a smooth, glossy surface in a calming turquoise color. It features a small golden ball at the bottom and a gold loop at the top for attachment. The star shape often symbolizes guidance, hope, and inspiration, while the turquoise color evokes tranquility and protection. The gold accents add a touch of elegance and luxury to the design.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>star pendant, turquoise, gold accents, glossy finish, layered design, small charm, jewelry accessory</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวที่มีพื้นผิวเรียบและเงางามในสีฟ้าเทอร์ควอยซ์ที่ให้ความรู้สึกสงบ มีลูกบอลทองเล็ก ๆ ที่ด้านล่างและห่วงทองที่ด้านบนสำหรับการติดตั้ง รูปดาวมักสื่อถึงการนำทาง ความหวัง และแรงบันดาลใจ สีฟ้าเทอร์ควอยซ์สื่อถึงความสงบและการปกป้อง ส่วนประกอบทองเพิ่มความหรูหราและสง่างามให้กับดีไซน์</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>star pendant, turquoise, gold accents, jewelry, glossy, elegant, symbolic, calming, small charm</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>จี้รูปดาว, สีฟ้าเทอร์ควอยซ์, ทอง, เครื่องประดับ, เงางาม, หรูหรา, สัญลักษณ์, สงบ, จี้เล็ก</t>
         </is>
       </c>
     </row>
@@ -490,12 +510,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>This elegant pendant features a star-shaped blue stone with a smooth, polished surface. It is accented by a gold-tone loop and a small gold ball at the bottom, creating a stylish and modern accessory perfect for adding a pop of color to any outfit.</t>
+          <t>This product is a star-shaped pendant with a smooth, glossy blue surface. It features a gold loop at the top for attachment and a small gold bead at the bottom, adding elegance and contrast. The star shape often symbolizes guidance and hope, while the blue color can represent calmness and stability. The gold accents enhance its luxurious and refined appearance.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>blue star, pendant, gold accents, polished stone, jewelry, modern design, accessory, small charm</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวที่มีพื้นผิวเรียบและมันวาวสีฟ้า มีห่วงทองที่ด้านบนสำหรับแขวนและลูกปัดทองเล็ก ๆ ที่ด้านล่าง เพิ่มความหรูหราและความโดดเด่น รูปดาวมักสื่อถึงการนำทางและความหวัง ส่วนสีฟ้าสื่อถึงความสงบและความมั่นคง ส่วนประกอบทองช่วยเพิ่มความหรูหราและความประณีต</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>star pendant, blue, gold accents, jewelry, glossy, elegant, symbolic, calm, luxury</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>จี้รูปดาว, สีฟ้า, ทอง, เครื่องประดับ, มันวาว, หรูหรา, สัญลักษณ์, สงบ, ความประณีต</t>
         </is>
       </c>
     </row>
@@ -512,12 +542,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features a polished, four-point star design with smooth, reflective surfaces. The pendant is attached to a sturdy circular loop, making it easy to add to any chain or bracelet. Its modern and minimalist style offers a versatile accessory for various occasions.</t>
+          <t>This product is a polished gold pendant shaped like a four-pointed star with smooth, rounded edges and a slightly raised center. The shiny gold color symbolizes luxury and elegance. The star shape often represents guidance, hope, and inspiration, making this pendant a meaningful accessory with a modern and refined aesthetic.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>gold, pendant, star, polished, minimalist, jewelry, accessory, shiny</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปดาวสี่แฉกที่มีขอบโค้งมนและส่วนกลางนูนเล็กน้อย สีทองเงางามสื่อถึงความหรูหราและสง่างาม รูปดาวมักสื่อถึงการนำทาง ความหวัง และแรงบันดาลใจ ทำให้จี้นี้เป็นเครื่องประดับที่มีความหมายพร้อมดีไซน์ทันสมัยและประณีต</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>gold pendant, star shape, four-pointed star, luxury, elegant, shiny, jewelry, symbolic, modern design</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปดาว, ดาวสี่แฉก, หรูหรา, สง่างาม, เงางาม, เครื่องประดับ, มีความหมาย, ดีไซน์ทันสมัย</t>
         </is>
       </c>
     </row>
@@ -534,12 +574,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>This elegant gold star-shaped pendant features eight pointed rays radiating from a central clear gemstone. The polished finish enhances its sophisticated look, making it a perfect accessory for adding a touch of sparkle and celestial charm to any jewelry collection.</t>
+          <t>This product is a gold pendant shaped like an eight-pointed star with a central clear gemstone. The pendant has a polished, shiny finish with smooth, elongated points radiating symmetrically from the center. The gold color symbolizes wealth and elegance, while the star shape often represents guidance, hope, and protection in various cultures.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>gold pendant, star shape, clear gemstone, eight points, polished finish, celestial design, jewelry charm, elegant accessory</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปดาวแปดแฉกที่มีอัญมณีใสตรงกลาง จี้มีผิวเรียบเงางามและปลายแฉกยาวที่กระจายออกจากศูนย์กลางอย่างสมมาตร สีทองสื่อถึงความมั่งคั่งและความสง่างาม ขณะที่รูปดาวมักหมายถึงการนำทาง ความหวัง และการปกป้องในวัฒนธรรมต่างๆ</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>gold pendant, star shape, eight points, clear gemstone, shiny finish, elegant jewelry, symbolic, guidance, hope, protection</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปดาว, แปดแฉก, อัญมณีใส, เงางาม, เครื่องประดับหรู, สัญลักษณ์, นำทาง, ความหวัง, การปกป้อง</t>
         </is>
       </c>
     </row>
@@ -556,12 +606,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features a unique starburst design with smooth, polished surfaces. At its center, a sparkling clear gemstone adds a touch of brilliance. The pendant includes a circular loop for easy attachment to chains or bracelets, making it a versatile accessory for any jewelry collection.</t>
+          <t>This product is a gold pendant shaped like a stylized star with four elongated points. It features a central clear gemstone that adds sparkle and elegance. The gold color symbolizes wealth and luxury, while the star shape often represents guidance, hope, and inspiration. The smooth, polished surface enhances its refined and modern aesthetic, making it a striking accessory.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>gold, pendant, starburst, gemstone, polished, jewelry, accessory, loop</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปดาวสี่แฉกที่ยาวเรียว มีอัญมณีใสตรงกลางเพิ่มความระยิบระยับและความหรูหรา สีทองสื่อถึงความมั่งคั่งและความหรูหรา รูปดาวมักสื่อถึงการนำทาง ความหวัง และแรงบันดาลใจ พื้นผิวเรียบเงาช่วยเพิ่มความทันสมัยและดูดี เหมาะเป็นเครื่องประดับที่โดดเด่น</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>gold pendant, star shape, gemstone, luxury, elegant, jewelry, shine, modern, accessory</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปดาว, อัญมณี, หรูหรา, สง่างาม, เครื่องประดับ, แวววาว, ทันสมัย, เครื่องประดับ</t>
         </is>
       </c>
     </row>
@@ -578,12 +638,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features a rectangular shape with softly rounded edges and a textured surface. At its center, a sparkling clear gemstone is set within a star-shaped engraving, adding a refined and sophisticated touch. The pendant includes a circular loop for easy attachment to a chain or bracelet.</t>
+          <t>This product is a small, rectangular gold pendant with rounded edges and a loop at the top for attaching to a chain. It features a central star-shaped engraving with a sparkling clear gemstone embedded in the middle. The dominant color is a rich, shiny gold, symbolizing luxury and elegance, while the star motif often represents guidance and protection in various cultures.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>gold pendant, rectangular shape, textured surface, clear gemstone, star engraving, jewelry charm, loop attachment, elegant design</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปสี่เหลี่ยมผืนผ้าขนาดเล็ก มีขอบโค้งมนและห่วงด้านบนสำหรับแขวนกับสร้อยคอ ตรงกลางมีการสลักรูปดาวพร้อมฝังอัญมณีใสประกายแวววาว สีหลักคือทองเงางามที่สื่อถึงความหรูหราและสง่างาม รูปดาวมีความหมายถึงการนำทางและการปกป้องในหลายวัฒนธรรม</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>gold pendant, rectangular, star motif, gemstone, luxury, jewelry, elegant, shiny, protective symbol</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>จี้ทอง, สี่เหลี่ยมผืนผ้า, รูปดาว, อัญมณี, หรูหรา, เครื่องประดับ, สง่างาม, เงางาม, สัญลักษณ์ปกป้อง</t>
         </is>
       </c>
     </row>
@@ -600,12 +670,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>This elegant gold heart-shaped pendant features a polished finish and a central blue gemstone set within a sunburst design. The pendant includes a sturdy gold loop for easy attachment to chains or bracelets, combining classic charm with a touch of vibrant color for versatile wear.</t>
+          <t>This product is a heart-shaped gold pendant featuring a central blue gemstone surrounded by a sunburst design. The smooth, polished gold surface contrasts beautifully with the deep blue gem, symbolizing love and protection. The sun motif often represents energy and life, making this pendant a meaningful accessory with elegant and timeless appeal.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>gold pendant, heart shape, blue gemstone, sunburst design, polished finish, jewelry charm, gold loop, elegant accessory</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปหัวใจสีทองที่มีอัญมณีสีน้ำเงินตรงกลางล้อมรอบด้วยลวดลายรูปดวงอาทิตย์ ผิวทองที่เรียบและเงางามตัดกับอัญมณีสีน้ำเงินเข้มอย่างสวยงาม สัญลักษณ์ดวงอาทิตย์มักแทนพลังงานและชีวิต ทำให้จี้นี้เป็นเครื่องประดับที่มีความหมายและดูสง่างามเหนือกาลเวลา</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>heart pendant, gold jewelry, blue gemstone, sunburst design, love symbol, elegant accessory, timeless, polished gold, meaningful</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>จี้รูปหัวใจ, เครื่องประดับทอง, อัญมณีสีน้ำเงิน, ลายดวงอาทิตย์, สัญลักษณ์ความรัก, เครื่องประดับหรู, เหนือกาลเวลา, ทองเงางาม, มีความหมาย</t>
         </is>
       </c>
     </row>
@@ -622,12 +702,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features a smooth, polished eye-shaped design with a radiant star engraving at its center. A sparkling clear gemstone is set within the star, adding a touch of brilliance. The pendant includes a sturdy circular loop for easy attachment to chains or bracelets.</t>
+          <t>This product is a gold pendant shaped like an eye with a smooth, polished surface. At the center, there is a starburst design engraved around a clear, sparkling gemstone. The gold color dominates the piece, symbolizing wealth and protection, while the eye shape often represents vigilance and warding off negative energy in various cultures.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>gold pendant, eye shape, star engraving, clear gemstone, polished finish, jewelry charm, circular loop, elegant design</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปทรงดวงตาที่มีพื้นผิวเรียบและเงางาม ตรงกลางมีลวดลายดาวที่สลักรอบอัญมณีใสที่เปล่งประกาย สีทองเป็นสีหลักของชิ้นงาน สื่อถึงความมั่งคั่งและการปกป้อง ขณะที่รูปทรงดวงตาสื่อถึงความระมัดระวังและการปัดเป่าพลังงานลบในหลายวัฒนธรรม</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>gold pendant, eye shape, starburst, gemstone, polished, protection, vigilance, jewelry, symbolic</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปดวงตา, ลวดลายดาว, อัญมณี, เงางาม, ปกป้อง, ระมัดระวัง, เครื่องประดับ, สัญลักษณ์</t>
         </is>
       </c>
     </row>
@@ -644,12 +734,22 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>This elegant gold star pendant features a textured, radiating pattern with a beaded border. The polished finish enhances its luxurious appeal, making it a versatile accessory for necklaces or charms. Its classic star shape and loop at the top allow for easy attachment to various jewelry pieces.</t>
+          <t>This product is a gold star-shaped pendant with a textured, radiating pattern in the center and a beaded border around the edges. The shiny gold color gives it a luxurious and elegant appearance. Stars often symbolize guidance, hope, and achievement, making this pendant a meaningful accessory or gift item.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>gold, star, pendant, beaded, textured, shiny, jewelry, charm</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวสีทองที่มีลวดลายลึกตรงกลางและขอบประดับด้วยเม็ดลูกปัด สีทองเงางามให้ความรู้สึกหรูหราและสง่างาม ดาวมักสื่อถึงการนำทาง ความหวัง และความสำเร็จ ทำให้จี้นี้เป็นเครื่องประดับหรือของขวัญที่มีความหมาย</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>gold, star, pendant, jewelry, beaded, textured, shiny, elegant, symbolic</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ทอง, ดาว, จี้, เครื่องประดับ, เม็ดลูกปัด, ลวดลาย, เงางาม, หรูหรา, มีความหมาย</t>
         </is>
       </c>
     </row>
@@ -666,12 +766,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>This gold-tone sun-shaped pendant features a stylized face with two sparkling crystal eyes. The design is smooth and polished, with radiating sun rays and a small loop for attaching to a chain. Its modern, artistic look makes it a striking accessory for any jewelry collection.</t>
+          <t>This product is a gold pendant shaped like a stylized sun with radiating spikes. It features a simple face design with two sparkling clear stones representing the eyes. The gold color dominates, giving it a luxurious and warm appearance. The sun motif often symbolizes energy, vitality, and life, making this pendant both a fashionable and meaningful accessory.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>gold pendant, sun design, crystal eyes, stylized face, radiant rays, polished finish, jewelry charm, modern accessory</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปดวงอาทิตย์ที่มีลักษณะเป็นแฉกแผ่ออกมา มีการออกแบบใบหน้าอย่างเรียบง่ายโดยใช้หินใสประกายสองเม็ดแทนดวงตา สีทองเป็นสีหลักที่ให้ความรู้สึกหรูหราและอบอุ่น รูปแบบดวงอาทิตย์มักสื่อถึงพลังงาน ความมีชีวิตชีวา และชีวิต ทำให้จี้นี้เป็นเครื่องประดับที่ทั้งสวยงามและมีความหมาย</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>gold pendant, sun shape, stylized face, sparkling stones, luxury jewelry, symbolic, energy, vitality, fashion accessory</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปดวงอาทิตย์, ใบหน้าเรียบง่าย, หินประกาย, เครื่องประดับหรู, สัญลักษณ์, พลังงาน, ชีวิตชีวา, เครื่องประดับแฟชั่น</t>
         </is>
       </c>
     </row>
@@ -688,12 +798,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features a crescent moon design with a detailed human face profile. The polished finish enhances its smooth curves and reflective surface, making it a striking accessory for any jewelry collection. The pendant includes a sturdy loop for easy attachment to chains or bracelets.</t>
+          <t>This product is a gold pendant shaped like a crescent moon with a serene human face carved into its curve. The dominant color is a shiny, reflective gold, symbolizing wealth, luxury, and timeless elegance. The crescent moon often represents growth and change, while the human face adds a mystical, celestial quality, evoking themes of night, dreams, and introspection.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>gold, crescent moon, face design, pendant, jewelry, polished, smooth, reflective</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปพระจันทร์เสี้ยวที่มีใบหน้ามนุษย์ที่สงบสลักอยู่บนเส้นโค้ง สีหลักคือสีทองเงางามที่สะท้อนแสง สื่อถึงความมั่งคั่ง หรูหรา และความคลาสสิก พระจันทร์เสี้ยวมักหมายถึงการเติบโตและการเปลี่ยนแปลง ส่วนใบหน้ามนุษย์เพิ่มความลึกลับและความเป็นสากล สื่อถึงคืน ฝัน และการไตร่ตรอง</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>gold pendant, crescent moon, face carving, jewelry, luxury, celestial, mystical, elegant, symbolic</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>จี้ทอง, พระจันทร์เสี้ยว, สลักใบหน้า, เครื่องประดับ, หรูหรา, สากล, ลึกลับ, สง่างาม, สัญลักษณ์</t>
         </is>
       </c>
     </row>
@@ -710,12 +830,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>This charming gold pendant features a polished star shape with a cut-out smiley face design. The smooth, reflective surface and rounded edges give it a sleek and modern look. Attached to a sturdy gold loop, it is perfect for adding a playful yet elegant touch to any necklace or bracelet.</t>
+          <t>This product is a gold-colored star-shaped pendant with a smooth, polished surface. It features a cheerful smiley face cutout with oval eyes and a curved mouth, giving it a playful and positive vibe. The star shape often symbolizes excellence and aspiration, while the smiley face adds a friendly and uplifting touch, making it a charming accessory for everyday wear.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>gold, star, smiley, pendant, polished, jewelry, charm, modern</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวสีทองที่มีพื้นผิวเรียบและเงางาม มีรูปหน้ายิ้มที่เจาะเป็นรูตาไข่และปากโค้ง ทำให้ดูสนุกสนานและมีพลังบวก รูปดาวมักสื่อถึงความเป็นเลิศและความมุ่งมั่น ขณะที่หน้ายิ้มเพิ่มความเป็นมิตรและความสดใส ทำให้เป็นเครื่องประดับที่น่ารักสำหรับใส่ในชีวิตประจำวัน</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>star pendant, gold color, smiley face, jewelry, charm, accessory, polished, playful, positive, fashion</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>จี้ดาว, สีทอง, หน้ายิ้ม, เครื่องประดับ, เสน่ห์, เครื่องแต่งกาย, เงางาม, สนุกสนาน, บวก, แฟชั่น</t>
         </is>
       </c>
     </row>
@@ -732,12 +862,22 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>This elegant star-shaped pendant features a polished gold-tone metal frame with a smooth, glossy purple enamel center. The pendant includes a sturdy gold-tone loop for easy attachment to necklaces or bracelets, combining playful charm with a refined finish for versatile wear.</t>
+          <t>This product is a star-shaped pendant with a smooth, glossy purple center encased in a shiny gold frame. The pendant has a small gold loop at the top for attaching to a chain or bracelet. The star shape often symbolizes guidance, hope, and inspiration, while the gold color adds a sense of luxury and elegance. The purple center adds a touch of creativity and spirituality to the design.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>star pendant, gold-tone, purple enamel, glossy finish, jewelry charm, accessory, fashion, elegant</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวที่มีส่วนกลางสีม่วงเงางามล้อมรอบด้วยกรอบทองเงาวาว จี้มีห่วงทองเล็ก ๆ ที่ด้านบนสำหรับแขวนกับสร้อยคอหรือสร้อยข้อมือ รูปดาวมักสื่อถึงการนำทาง ความหวัง และแรงบันดาลใจ ส่วนสีทองเพิ่มความหรูหราและสง่างาม สีม่วงตรงกลางเพิ่มความคิดสร้างสรรค์และความเป็นจิตวิญญาณให้กับดีไซน์</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>star pendant, gold frame, purple center, jewelry, luxury, elegant, creative, spiritual, gift, fashion</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>จี้รูปดาว, กรอบทอง, สีม่วง, เครื่องประดับ, หรูหรา, สง่างาม, สร้างสรรค์, จิตวิญญาณ, ของขวัญ, แฟชั่น</t>
         </is>
       </c>
     </row>
@@ -754,12 +894,22 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features an oval shape with a raised infinity symbol at its center. Surrounding the infinity are embossed celestial motifs including stars, a crescent moon, and small dots, all set against a textured background. The pendant has a polished finish and a sturdy loop for easy attachment.</t>
+          <t>This product is a gold-colored oval pendant featuring an infinity symbol at its center. Surrounding the infinity are various star shapes and a crescent moon, all embossed in the same gold tone. The design suggests themes of eternity, cosmic energy, and celestial beauty, making it a meaningful accessory with spiritual and symbolic significance.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>gold pendant, oval shape, infinity symbol, celestial design, stars, crescent moon, textured background, polished finish</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปวงรีสีทอง มีสัญลักษณ์อินฟินิตี้อยู่ตรงกลาง รอบๆ มีรูปดาวและพระจันทร์เสี้ยวที่นูนขึ้นในโทนสีทองเดียวกัน การออกแบบนี้สื่อถึงความเป็นนิรันดร์ พลังจักรวาล และความงามของท้องฟ้า เหมาะเป็นเครื่องประดับที่มีความหมายทางจิตวิญญาณและสัญลักษณ์ที่ลึกซึ้ง</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>gold pendant, oval shape, infinity symbol, crescent moon, stars, celestial, spiritual, jewelry, symbolic, cosmic</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปวงรี, สัญลักษณ์อินฟินิตี้, พระจันทร์เสี้ยว, ดาว, จักรวาล, จิตวิญญาณ, เครื่องประดับ, สัญลักษณ์, ความหมาย</t>
         </is>
       </c>
     </row>
@@ -776,12 +926,22 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>This round pendant features a textured gray background encased in a polished gold frame. It showcases a gold sun with a vibrant red gemstone center, a crescent moon, and three small gold dots, creating a celestial theme. The pendant has a smooth gold bail for easy attachment to a chain.</t>
+          <t>This round pendant features a gold frame with a textured gray background. It showcases a golden sun with a central red gemstone and a crescent moon, symbolizing the balance between day and night. The design is elegant and mystical, combining warm gold tones with the striking red gem to create a piece that evokes celestial harmony and timeless beauty.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>gold pendant, celestial design, red gemstone, sun and moon, textured background, round shape, jewelry charm, polished finish</t>
+          <t>จี้ทรงกลมนี้มีกรอบทองและพื้นหลังสีเทาที่มีลวดลาย มีรูปพระอาทิตย์สีทองพร้อมอัญมณีสีแดงตรงกลางและพระจันทร์เสี้ยว สื่อถึงความสมดุลระหว่างกลางวันและกลางคืน การออกแบบดูสง่างามและลึกลับ ผสมผสานโทนสีทองอบอุ่นกับอัญมณีสีแดงที่โดดเด่น สร้างชิ้นงานที่สื่อถึงความกลมกลืนของจักรวาลและความงามเหนือกาลเวลา</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>pendant, gold, sun, moon, red gemstone, celestial, round, jewelry, mystical, balance</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>จี้, ทอง, พระอาทิตย์, พระจันทร์, อัญมณีแดง, จักรวาล, ทรงกลม, เครื่องประดับ, ลึกลับ, สมดุล</t>
         </is>
       </c>
     </row>
@@ -798,12 +958,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>This elegant rectangular pendant features a deep blue enamel background with a polished gold crescent moon and three stars. The border is detailed with a textured gold frame, and the words 'THE MOON' are embossed in gold at the bottom, creating a celestial and sophisticated accessory.</t>
+          <t>This rectangular pendant features a deep blue background with a gold crescent moon and three stars, symbolizing night and mystery. The gold frame and details add a luxurious touch, while the inscription 'THE MOON' emphasizes its celestial theme. The combination of blue and gold evokes a sense of elegance and cosmic wonder, often associated with intuition and dreams.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>pendant, gold, blue enamel, crescent moon, stars, rectangular, celestial, textured frame</t>
+          <t>จี้รูปสี่เหลี่ยมผืนผ้าชิ้นนี้มีพื้นหลังสีน้ำเงินเข้มพร้อมพระจันทร์เสี้ยวและดาวสามดวงสีทอง สื่อถึงความลึกลับและยามค่ำคืน กรอบและรายละเอียดสีทองเพิ่มความหรูหรา พร้อมคำว่า 'THE MOON' ที่เน้นธีมดวงดาว การผสมผสานระหว่างสีน้ำเงินและทองสร้างความรู้สึกสง่างามและความมหัศจรรย์ของจักรวาล ซึ่งมักเกี่ยวข้องกับสัญชาตญาณและความฝัน</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>pendant, moon, stars, gold, blue, celestial, elegant, mystical, jewelry</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>จี้, พระจันทร์, ดาว, ทอง, น้ำเงิน, จักรวาล, หรูหรา, ลึกลับ, เครื่องประดับ</t>
         </is>
       </c>
     </row>
@@ -820,12 +990,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features a planet design with a smooth circular base and a ring encircling it. The surface is adorned with star-shaped engravings and sparkling clear gemstones, adding a celestial and luxurious touch. The pendant includes a sturdy loop for easy attachment to chains or bracelets.</t>
+          <t>This product is a gold pendant shaped like a planet with rings, featuring a smooth circular form. It is adorned with small sparkling stones arranged as stars and along the rings, adding a celestial and elegant touch. The dominant color is shiny gold, symbolizing luxury and timeless beauty, while the star motifs evoke a sense of wonder and cosmic inspiration.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>gold pendant, planet design, star engravings, clear gemstones, celestial jewelry, circular charm, luxury accessory, jewelry loop</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปดาวเคราะห์ที่มีวงแหวนล้อมรอบ มีรูปทรงกลมเรียบเนียน ประดับด้วยหินประกายเล็กๆ ที่จัดวางเป็นรูปดาวและตามวงแหวน เพิ่มความรู้สึกของจักรวาลและความหรูหรา สีหลักคือสีทองเงางาม สื่อถึงความหรูหราและความงามเหนือกาลเวลา ส่วนลวดลายดาวสื่อถึงความมหัศจรรย์และแรงบันดาลใจจากจักรวาล</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>gold pendant, planet shape, celestial, stars, rings, sparkling stones, luxury, elegant, cosmic</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปดาวเคราะห์, จักรวาล, ดาว, วงแหวน, หินประกาย, หรูหรา, สง่างาม, จักรวาล</t>
         </is>
       </c>
     </row>
@@ -842,12 +1022,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features a shooting star design with a central clear gemstone in the star and multiple smaller sparkling stones adorning the trailing tail. The polished gold finish adds a luxurious shine, making it a perfect accessory for a refined and celestial-inspired look.</t>
+          <t>This product is a gold pendant shaped like a shooting star. It features a five-pointed star with a central clear gemstone and a trailing tail adorned with multiple small sparkling stones. The dominant color is a rich gold, symbolizing luxury and elegance, while the star motif often represents guidance, hope, and inspiration in various cultures.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>gold, pendant, shooting star, gemstones, sparkling, jewelry, luxury, celestial</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปดาวตก มีดาวห้าแฉกที่มีอัญมณีใสตรงกลางและหางที่ประดับด้วยหินเล็กๆ หลายเม็ด สีหลักคือทองที่แสดงถึงความหรูหราและสง่างาม รูปดาวสื่อถึงการนำทาง ความหวัง และแรงบันดาลใจในหลายวัฒนธรรม</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>gold pendant, shooting star, star charm, gemstone, luxury jewelry, sparkling stones, elegant, symbolic, hope, inspiration</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>จี้ทอง, ดาวตก, จี้รูปดาว, อัญมณี, เครื่องประดับหรู, หินประกาย, สง่างาม, สัญลักษณ์, ความหวัง, แรงบันดาลใจ</t>
         </is>
       </c>
     </row>
@@ -864,12 +1054,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>This elegant star-shaped pendant features a polished gold-tone finish adorned with multiple sparkling clear crystals. The pendant includes a sturdy loop for easy attachment to chains or bracelets, making it a versatile and stylish accessory for any jewelry collection.</t>
+          <t>This product is a star-shaped pendant crafted in gold with a smooth, polished finish. The star is adorned with numerous small, sparkling clear stones, likely diamonds or cubic zirconia, embedded within the gold frame. The golden color symbolizes luxury and warmth, while the star shape often represents guidance, hope, and inspiration, making it a meaningful and elegant accessory.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>star, gold-tone, crystals, pendant, jewelry, sparkling, accessory, elegant</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวที่ทำจากทองคำขัดเงาอย่างเรียบเนียน ดาวประดับด้วยหินใสเล็ก ๆ จำนวนมากซึ่งอาจเป็นเพชรหรือซูริเนียมฝังอยู่ในกรอบทอง สีทองสื่อถึงความหรูหราและความอบอุ่น รูปดาวมักสื่อถึงการนำทาง ความหวัง และแรงบันดาลใจ ทำให้เป็นเครื่องประดับที่มีความหมายและสง่างาม</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>star pendant, gold jewelry, sparkling stones, luxury accessory, elegant design, symbolic shape, gift idea, fashion jewelry</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>จี้รูปดาว, เครื่องประดับทอง, หินประกาย, เครื่องประดับหรู, ดีไซน์สง่างาม, รูปทรงสัญลักษณ์, ของขวัญ, แฟชั่น</t>
         </is>
       </c>
     </row>
@@ -886,12 +1086,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>This elegant star-shaped pendant features a smooth, polished gold-tone finish with a sleek, modern design. Its five-pointed star form is complemented by a sturdy loop for easy attachment to chains or bracelets, making it a versatile accessory for various jewelry styles.</t>
+          <t>This product is a polished gold star-shaped pendant with a smooth, reflective surface. The star has five points and a small loop at the top for attaching to a chain or bracelet. The golden color symbolizes wealth, success, and positivity, often associated with achievement and guidance. Its sleek and simple design makes it a versatile accessory for various styles.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>gold, star, pendant, jewelry, polished, metal, accessory, modern</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวสีทองเงางาม มีพื้นผิวเรียบและสะท้อนแสง ดาวมีห้าจุดและมีห่วงเล็ก ๆ ที่ด้านบนสำหรับใส่กับสร้อยคอหรือสร้อยข้อมือ สีทองสื่อถึงความมั่งคั่ง ความสำเร็จ และความเป็นบวก ซึ่งมักเกี่ยวข้องกับความสำเร็จและการนำทาง การออกแบบที่เรียบง่ายและทันสมัยทำให้เหมาะกับสไตล์หลากหลายแบบ</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>gold, star, pendant, jewelry, shine, accessory, simple, elegant, symbolic</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>ทอง, ดาว, จี้, เครื่องประดับ, เงางาม, อุปกรณ์เสริม, เรียบง่าย, สง่างาม, สัญลักษณ์</t>
         </is>
       </c>
     </row>
@@ -908,12 +1118,22 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>This elegant star-shaped pendant features a smooth white enamel surface bordered by a polished gold frame. At its center, a sparkling clear gemstone adds a touch of brilliance. The pendant is attached to a shiny gold loop, perfect for adding charm to any necklace or bracelet.</t>
+          <t>This pendant features a star-shaped design with a smooth white enamel surface bordered by a shiny gold frame. At the center, a sparkling clear gemstone adds elegance and brilliance. The star shape often symbolizes guidance, hope, and inspiration, making this piece both stylish and meaningful. The combination of white, gold, and the gemstone creates a luxurious and timeless look.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>star, pendant, gold, white enamel, gemstone, jewelry, charm, shine</t>
+          <t>จี้รูปดาวนี้มีดีไซน์เป็นรูปดาวที่มีพื้นผิวเคลือบอีนาเมลสีขาวเรียบล้อมรอบด้วยกรอบทองเงางาม ตรงกลางประดับด้วยอัญมณีใสที่เปล่งประกายเพิ่มความหรูหราและโดดเด่น รูปดาวมักสื่อถึงการนำทาง ความหวัง และแรงบันดาลใจ ทำให้ชิ้นนี้ทั้งสวยงามและมีความหมาย การผสมผสานของสีขาว ทอง และอัญมณีสร้างลุคที่หรูหราและคลาสสิก</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>star pendant, gold frame, white enamel, clear gemstone, luxury jewelry, symbolic, elegant, shiny, timeless, inspiration</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>จี้รูปดาว, กรอบทอง, อีนาเมลสีขาว, อัญมณีใส, เครื่องประดับหรู, มีความหมาย, สง่างาม, เงางาม, คลาสสิก, แรงบันดาลใจ</t>
         </is>
       </c>
     </row>
@@ -930,12 +1150,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>This elegant crescent moon pendant features a polished gold-tone frame with a deep blue enamel inlay. A single clear gemstone is set near the center, adding a subtle sparkle. The pendant includes a smooth, rounded bail for easy attachment to chains or bracelets, combining celestial charm with refined craftsmanship.</t>
+          <t>This pendant features a crescent moon shape with a smooth, deep blue enamel surface bordered by polished gold. A small, clear gemstone is embedded near the center, adding a touch of sparkle. The crescent moon often symbolizes growth and change, while the blue and gold colors evoke a sense of elegance and celestial beauty.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>crescent moon, gold-tone, blue enamel, gemstone, pendant, jewelry, celestial, charm</t>
+          <t>จี้นี้มีรูปทรงพระจันทร์เสี้ยวที่มีพื้นผิวเคลือบสีน้ำเงินเข้มเรียบเนียน ขอบทองเงางาม ประดับด้วยอัญมณีใสขนาดเล็กที่ฝังอยู่ใกล้กลางจี้ เพิ่มความระยิบระยับ พระจันทร์เสี้ยวมักสื่อถึงการเติบโตและการเปลี่ยนแปลง สีฟ้าและทองให้ความรู้สึกหรูหราและงดงามเหมือนดวงดาวในท้องฟ้า</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>crescent moon, pendant, blue enamel, gold border, gemstone, jewelry, elegant, celestial, charm</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>พระจันทร์เสี้ยว, จี้, เคลือบสีน้ำเงิน, ขอบทอง, อัญมณี, เครื่องประดับ, หรูหรา, ท้องฟ้า, เครื่องราง</t>
         </is>
       </c>
     </row>
@@ -952,12 +1182,22 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>This gold-toned pendant features a textured, eight-pointed star design with a slightly hammered finish. The pendant includes a circular loop at the top for easy attachment to chains or bracelets, combining a modern aesthetic with a celestial-inspired motif for versatile jewelry styling.</t>
+          <t>This product is a gold-colored pendant shaped like an eight-pointed star with a textured surface. The star design symbolizes guidance, protection, and illumination in many cultures. Its shiny metallic finish adds a luxurious and elegant touch, making it suitable for jewelry or decorative accessories. The loop at the top allows it to be easily attached to chains or cords.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>gold pendant, star shape, textured finish, eight points, hammered metal, jewelry charm, celestial design, loop attachment</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้สีทองรูปดาวแปดแฉกที่มีพื้นผิวขรุขระ รูปดาวนี้สื่อถึงการนำทาง การปกป้อง และแสงสว่างในหลายวัฒนธรรม ผิวโลหะมันวาวเพิ่มความหรูหราและสง่างาม เหมาะสำหรับเครื่องประดับหรือของตกแต่ง ห่วงด้านบนช่วยให้สามารถแขวนกับสร้อยหรือสายได้ง่าย</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>gold pendant, star shape, eight points, textured surface, jewelry charm, metallic finish, luxury accessory, symbolic design</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปดาว, แปดแฉก, พื้นผิวขรุขระ, เครื่องประดับ, ผิวโลหะ, ของตกแต่ง, สัญลักษณ์</t>
         </is>
       </c>
     </row>
@@ -974,12 +1214,22 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>This elegant gold sun pendant features a detailed, expressive face at its center, surrounded by twelve smooth, curved rays. The polished finish enhances its radiant appearance, making it a striking accessory for necklaces or keychains. A circular loop at the top allows easy attachment.</t>
+          <t>This product is a golden sun-shaped pendant featuring a human face at its center. The sun rays are stylized with smooth, rounded edges radiating outward. The dominant color is a shiny gold, symbolizing warmth, energy, and life. The facial expression is calm and serene, evoking a sense of peace and positivity often associated with sun imagery in various cultures.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>gold, sun, pendant, face, rays, shiny, jewelry, accessory</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดวงอาทิตย์สีทองที่มีใบหน้ามนุษย์อยู่ตรงกลาง รังสีของดวงอาทิตย์ถูกออกแบบให้มีขอบโค้งมนและเรียบเนียนแผ่ออกไป สีหลักคือสีทองเงางาม ซึ่งสื่อถึงความอบอุ่น พลังงาน และชีวิต ใบหน้ามีสีหน้าเงียบสงบและสงบสุข สื่อถึงความสงบและความรู้สึกบวกที่มักเกี่ยวข้องกับภาพลักษณ์ของดวงอาทิตย์ในวัฒนธรรมต่างๆ</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>sun pendant, gold jewelry, sun face, symbolic, warmth, energy, serene, radiant, cultural, metal charm</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>จี้ดวงอาทิตย์, เครื่องประดับทอง, ใบหน้าดวงอาทิตย์, สัญลักษณ์, อบอุ่น, พลังงาน, สงบ, แสงสว่าง, วัฒนธรรม, จี้โลหะ</t>
         </is>
       </c>
     </row>
@@ -996,12 +1246,22 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features an oval shape with a textured background. The design includes a stylized sun with a smiling face, surrounded by small raised dots and two leafy branches at the bottom. The pendant has a polished gold border and a sturdy loop for attaching to a chain.</t>
+          <t>This product is a gold pendant with an oval shape featuring a raised sun motif with a smiling face at its center. Surrounding the sun are small round dots and two leaf-like designs at the bottom, all embossed in gold. The warm gold color and sun imagery symbolize positivity, warmth, and life, often associated with good fortune and energy in various cultures.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>gold pendant, oval shape, sun design, textured background, leaf motifs, polished finish, jewelry charm, smiling face</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปวงรีที่มีลวดลายพระอาทิตย์นูนตรงกลางพร้อมใบหน้าที่ยิ้มล้อมรอบด้วยจุดกลมเล็ก ๆ และลายใบไม้สองข้างด้านล่าง สีทองอบอุ่นและภาพพระอาทิตย์สื่อถึงความสดใส ความอบอุ่น และชีวิต ซึ่งมักเกี่ยวข้องกับโชคลาภและพลังงานในหลายวัฒนธรรม</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>gold pendant, oval shape, sun motif, smiling face, leaf design, embossed, warm color, symbolic, positive energy</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปวงรี, ลายพระอาทิตย์, ใบหน้ายิ้ม, ลายใบไม้, นูน, สีทอง, สัญลักษณ์, พลังบวก</t>
         </is>
       </c>
     </row>
@@ -1018,12 +1278,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>This elegant gold star-shaped pendant features a textured inner star design with a sparkling round clear gemstone set at its center. The pendant includes a smooth, polished gold loop for easy attachment to chains or bracelets, combining classic charm with a modern touch.</t>
+          <t>This product is a gold star-shaped pendant with a smooth, polished finish. At the center of the star is a sparkling clear gemstone, adding elegance and brilliance. The gold color symbolizes wealth and luxury, while the star shape often represents guidance and hope. The pendant's simple yet refined design makes it suitable for various cultural and fashion contexts.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>gold pendant, star shape, textured design, clear gemstone, polished finish, jewelry charm, small loop, elegant accessory</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวสีทองที่มีผิวเรียบและเงางาม ตรงกลางดาวประดับด้วยอัญมณีใสที่เปล่งประกาย เพิ่มความหรูหราและโดดเด่น สีทองสื่อถึงความมั่งคั่งและความหรูหรา ส่วนรูปดาวมักสื่อถึงการนำทางและความหวัง การออกแบบที่เรียบง่ายแต่ประณีตนี้เหมาะกับบริบททางวัฒนธรรมและแฟชั่นหลากหลายแบบ</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>gold pendant, star shape, gemstone, jewelry, luxury, elegant, fashion, symbolic, shine, gift</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปดาว, อัญมณี, เครื่องประดับ, หรูหรา, สง่างาม, แฟชั่น, สัญลักษณ์, ประกาย, ของขวัญ</t>
         </is>
       </c>
     </row>
@@ -1040,12 +1310,22 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>This gold-tone pendant features a rectangular shape with rounded edges, adorned with embossed celestial motifs including an eye, crescent moons, and stars. The pendant has a smooth, polished finish with a textured background, creating a striking contrast. It includes a sturdy loop for easy attachment to chains or bracelets.</t>
+          <t>This product is a gold-colored pendant with a rectangular shape featuring slightly angled corners. The design includes a central eye surrounded by radiating lines, crescent moons, and stars, symbolizing protection, intuition, and celestial guidance. The shiny gold finish adds a luxurious and mystical feel, making it a meaningful accessory with spiritual and cosmic connotations.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>gold pendant, celestial design, eye motif, crescent moon, star accents, embossed texture, rectangular shape, jewelry charm</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้สีทองรูปทรงสี่เหลี่ยมผืนผ้าที่มีมุมเฉียงเล็กน้อย ลวดลายประกอบด้วยดวงตากลางล้อมรอบด้วยเส้นแผ่รังสี พระจันทร์เสี้ยว และดาว ซึ่งสื่อถึงการปกป้อง สัญชาตญาณ และการนำทางจากจักรวาล ผิวเคลือบทองเงางามเพิ่มความหรูหราและความลึกลับ ทำให้เป็นเครื่องประดับที่มีความหมายทางจิตวิญญาณและจักรวาล</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>gold pendant, rectangular shape, eye symbol, crescent moon, stars, spiritual, mystical, luxury, cosmic, protection</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปสี่เหลี่ยม, สัญลักษณ์ดวงตา, พระจันทร์เสี้ยว, ดาว, จิตวิญญาณ, ลึกลับ, หรูหรา, จักรวาล, ปกป้อง</t>
         </is>
       </c>
     </row>
@@ -1062,12 +1342,22 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>This elegant round pendant features a gold-tone frame with a soft pink enamel background divided into six sections. Each section contains a unique gold symbol, including an eye with a turquoise center, a horseshoe, a starburst, a wishbone, a pig, and the number seven. A clear gemstone is set in the center, adding a touch of sparkle.</t>
+          <t>This round pendant features a gold frame with a soft pink background divided into six sections, each containing a unique gold symbol including an eye, horseshoe, star, wishbone, pig, and the number seven. A clear gemstone is set in the center, adding elegance. The symbols suggest themes of luck, protection, and prosperity, commonly found in various cultural talismans.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>gold pendant, pink enamel, symbol charms, turquoise eye, clear gemstone, round jewelry, luck symbols, divided sections</t>
+          <t>จี้ทรงกลมนี้มีกรอบสีทองและพื้นหลังสีชมพูอ่อนแบ่งเป็นหกส่วน แต่ละส่วนมีสัญลักษณ์ทองคำที่ไม่ซ้ำกัน ได้แก่ ดวงตา เกือกม้า ดาว กระดูก wishbone หมู และเลขเจ็ด มีอัญมณีใสประดับตรงกลางเพิ่มความหรูหรา สัญลักษณ์เหล่านี้สื่อถึงโชคลาภ การปกป้อง และความมั่งคั่ง ซึ่งพบได้ในเครื่องรางวัฒนธรรมต่างๆ</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>pendant, gold, pink, luck, symbols, talisman, gemstone, protection, prosperity</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>จี้, ทอง, ชมพู, โชคลาภ, สัญลักษณ์, เครื่องราง, อัญมณี, ปกป้อง, มั่งคั่ง</t>
         </is>
       </c>
     </row>
@@ -1084,12 +1374,22 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>This elegant gold star-shaped pendant features a textured surface with a smaller star-shaped gemstone inset at its center. The polished finish enhances its luxurious appeal, making it a stylish accessory for various occasions. The pendant's loop allows easy attachment to chains or bracelets.</t>
+          <t>This product is a gold star-shaped pendant with a smooth, polished surface and a slightly textured design. It features a smaller star-shaped inset in the center, filled with a translucent material containing gold flakes. The star shape often symbolizes guidance, hope, and inspiration, while the gold color conveys luxury and elegance, making it a meaningful and stylish accessory.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>gold, star, pendant, textured, gemstone, jewelry, polished, accessory</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวสีทองที่มีพื้นผิวเรียบเงาและดีไซน์ที่มีลักษณะขรุขระเล็กน้อย ตรงกลางมีดาวรูปทรงเล็กกว่าฝังอยู่ภายในที่เต็มไปด้วยวัสดุโปร่งแสงพร้อมเศษทอง ดาวเป็นสัญลักษณ์ของการนำทาง ความหวัง และแรงบันดาลใจ สีทองสื่อถึงความหรูหราและสง่างาม ทำให้เป็นเครื่องประดับที่มีความหมายและดูดี</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>star pendant, gold jewelry, luxury accessory, polished finish, textured design, symbolic star, gold flakes, elegant, hope symbol, inspiration</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>จี้รูปดาว, เครื่องประดับทอง, เครื่องประดับหรู, พื้นผิวเงา, ดีไซน์ขรุขระ, ดาวสัญลักษณ์, เศษทอง, สง่างาม, สัญลักษณ์ความหวัง, แรงบันดาลใจ</t>
         </is>
       </c>
     </row>
@@ -1106,12 +1406,22 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>This elegant gold-tone pendant features a polished round disc with a bold blue star inset at its center. The smooth, reflective surface and vibrant color contrast create a modern and stylish accessory perfect for adding a touch of charm to any outfit.</t>
+          <t>This product is a round gold pendant featuring a prominent blue star in the center. The pendant has a smooth, polished surface with a shiny finish, highlighting the contrast between the rich gold and deep blue colors. The star symbol often represents guidance, hope, and aspiration, making this piece both visually appealing and meaningful.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>gold pendant, blue star, round disc, polished finish, modern design, charming accessory, jewelry, fashion</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปทรงกลมสีทองที่มีดาวสีน้ำเงินเด่นอยู่ตรงกลาง จี้มีพื้นผิวเรียบและเงางาม เน้นความแตกต่างระหว่างสีทองสดใสกับสีน้ำเงินเข้ม ดาวเป็นสัญลักษณ์ที่มักแทนความหวัง ความมุ่งมั่น และการนำทาง ทำให้ชิ้นนี้ดูสวยงามและมีความหมายในตัวเอง</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>pendant, gold, blue star, round, jewelry, shiny, symbolic, polished, accessory</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>จี้, ทอง, ดาวสีน้ำเงิน, ทรงกลม, เครื่องประดับ, เงางาม, สัญลักษณ์, เรียบ, อุปกรณ์เสริม</t>
         </is>
       </c>
     </row>
@@ -1128,12 +1438,22 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>This elegant star-shaped pendant features a polished gold-tone finish with three distinct gemstones embedded: a round pink stone, a marquise-shaped green stone, and a square green stone. The smooth, reflective surface and unique gemstone arrangement create a sophisticated and eye-catching accessory.</t>
+          <t>This product is a star-shaped pendant made of shiny gold metal. It features three embedded gemstones: a round pink gem at the top, a marquise-shaped green gem on the left, and a square green gem on the right. The star shape often symbolizes guidance and hope, while the gold color signifies luxury and warmth. The combination of colors and shapes gives it a charming and elegant appearance.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>star pendant, gold tone, pink gemstone, green gemstones, polished finish, unique design, jewelry accessory, elegant</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวทำจากโลหะสีทองเงางาม มีอัญมณีฝังสามเม็ด ได้แก่ เม็ดกลมสีชมพูด้านบน เม็ดรูปมาคีส์สีเขียวด้านซ้าย และเม็ดสี่เหลี่ยมสีเขียวด้านขวา รูปดาวมักสื่อถึงการนำทางและความหวัง ส่วนสีทองแสดงถึงความหรูหราและอบอุ่น การผสมผสานของสีและรูปทรงทำให้ดูน่ารักและสง่างาม</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>star pendant, gold, pink gem, green gem, jewelry, elegant, luxury, charming, gift</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>จี้รูปดาว, ทอง, อัญมณีชมพู, อัญมณีเขียว, เครื่องประดับ, สง่างาม, หรูหรา, น่ารัก, ของขวัญ</t>
         </is>
       </c>
     </row>
@@ -1150,12 +1470,22 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>This elegant pendant features a polished gold-tone star design with a smooth, reflective surface. The star has a three-dimensional, faceted structure that adds depth and sophistication. Attached to a circular loop, it is perfect for adding a touch of shine to any necklace or bracelet.</t>
+          <t>This product is a polished gold star-shaped pendant with a smooth, reflective surface. The star has four elongated points, giving it a modern and sleek appearance. The gold color symbolizes luxury, success, and warmth, often associated with positive energy and achievement. The pendant's simple yet elegant design makes it suitable for various cultural styles and personal adornment.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>gold, star, pendant, jewelry, shiny, faceted, elegant, accessory</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวสีทองเงางาม มีพื้นผิวเรียบและสะท้อนแสง ดาวมีปลายแหลมสี่ด้านยาว ทำให้ดูทันสมัยและเรียบหรู สีทองสื่อถึงความหรูหรา ความสำเร็จ และความอบอุ่น มักเชื่อมโยงกับพลังบวกและความสำเร็จ การออกแบบที่เรียบง่ายแต่สง่างามนี้เหมาะกับสไตล์วัฒนธรรมและการประดับตกแต่งส่วนตัวหลากหลายแบบ</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>gold pendant, star shape, jewelry, luxury, elegant, shine, fashion, accessory</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>จี้ทอง, รูปดาว, เครื่องประดับ, หรูหรา, สง่างาม, เงางาม, แฟชั่น, อุปกรณ์เสริม</t>
         </is>
       </c>
     </row>
@@ -1172,12 +1502,22 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>This elegant gold pendant features a polished star design with four elongated points and a smooth, reflective surface. The pendant includes a sturdy circular loop for easy attachment to chains or bracelets, making it a versatile and stylish accessory for any jewelry collection.</t>
+          <t>This product is a gold pendant shaped like a four-pointed star with a sleek, polished surface. The star's sharp, elongated points create a modern and elegant look. The gold color symbolizes wealth, luxury, and timeless beauty, often associated with high value and sophistication. The pendant's simple yet striking design makes it a versatile accessory for various styles.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>gold, star, pendant, jewelry, polished, reflective, loop, accessory</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้ทองรูปดาวสี่แฉกที่มีพื้นผิวเรียบเงางาม ปลายแหลมยาวของดาวสร้างรูปลักษณ์ที่ทันสมัยและสง่างาม สีทองสื่อถึงความมั่งคั่ง ความหรูหรา และความงามที่ไม่เสื่อมคลาย ซึ่งมักเชื่อมโยงกับมูลค่าสูงและความประณีต การออกแบบที่เรียบง่ายแต่โดดเด่นนี้ทำให้จี้เหมาะกับสไตล์หลากหลายแบบ</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>gold, pendant, star, jewelry, elegant, luxury, modern, shine, accessory</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>ทอง, จี้, ดาว, เครื่องประดับ, สง่างาม, หรูหรา, ทันสมัย, เงางาม, อุปกรณ์เสริม</t>
         </is>
       </c>
     </row>
@@ -1194,12 +1534,22 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>This elegant crescent moon pendant features a polished gold-tone frame with a white enamel interior adorned with blue star and dot accents. The smooth finish and delicate loop make it perfect for adding a celestial touch to any necklace or bracelet.</t>
+          <t>This product is a crescent moon-shaped pendant with a smooth gold outline. The interior is white with blue star and dot patterns, evoking a night sky theme. The crescent moon often symbolizes growth and change, while the stars add a whimsical, celestial touch. The combination of gold, white, and blue creates a delicate and elegant appearance suitable for jewelry lovers.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>crescent moon, gold-tone, white enamel, blue stars, pendant, celestial, jewelry charm, delicate</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปพระจันทร์เสี้ยวที่มีขอบทองเรียบเนียน ภายในเป็นสีขาวพร้อมลวดลายดาวและจุดสีฟ้า สื่อถึงธีมท้องฟ้ายามค่ำคืน พระจันทร์เสี้ยวมักสื่อถึงการเติบโตและการเปลี่ยนแปลง ส่วนดาวเพิ่มความรู้สึกน่ารักและเกี่ยวกับจักรวาล การผสมผสานของสีทอง ขาว และฟ้าทำให้ดูอ่อนโยนและสง่างาม เหมาะสำหรับคนรักเครื่องประดับ</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>crescent moon, pendant, gold, white, blue stars, celestial, jewelry, elegant, night sky, charm</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>พระจันทร์เสี้ยว, จี้, ทอง, สีขาว, ดาวสีฟ้า, จักรวาล, เครื่องประดับ, สง่างาม, ท้องฟ้ายามค่ำคืน, เครื่องราง</t>
         </is>
       </c>
     </row>
@@ -1216,12 +1566,22 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>This elegant gold heart-shaped pendant features a smooth, polished surface with a single sparkling clear gemstone set in the center. Its simple yet refined design makes it a timeless accessory suitable for everyday wear or special occasions.</t>
+          <t>This product is a heart-shaped pendant made of polished gold with a smooth, reflective surface. At its center, there is a small, sparkling diamond that adds elegance and luxury. The heart shape symbolizes love and affection, making this pendant a meaningful accessory for expressing emotions or celebrating special relationships. The warm gold tone enhances its classic and timeless appeal.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>gold, heart, pendant, gemstone, polished, jewelry, elegant, simple</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปหัวใจทำจากทองคำขัดเงา มีผิวเรียบและสะท้อนแสง ที่ตรงกลางมีเพชรเม็ดเล็กที่เปล่งประกายเพิ่มความหรูหรา รูปหัวใจสื่อถึงความรักและความผูกพัน ทำให้จี้นี้เป็นเครื่องประดับที่มีความหมายสำหรับการแสดงความรู้สึกหรือเฉลิมฉลองความสัมพันธ์พิเศษ สีทองอบอุ่นช่วยเพิ่มความคลาสสิกและความงดงามเหนือกาลเวลา</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>heart pendant, gold jewelry, diamond, love symbol, elegant, luxury, classic, timeless, polished, gift</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>จี้รูปหัวใจ, เครื่องประดับทอง, เพชร, สัญลักษณ์ความรัก, หรูหรา, คลาสสิก, เหนือกาลเวลา, ขัดเงา, ของขวัญ, สง่างาม</t>
         </is>
       </c>
     </row>
@@ -1238,12 +1598,22 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>This elegant star-shaped charm features a polished gold-tone frame with a vibrant turquoise enamel center speckled with subtle glitter. A smaller gold star embellishment sits in the middle, adding a delicate touch. The charm includes a sturdy gold loop for easy attachment to bracelets or necklaces.</t>
+          <t>This product is a star-shaped pendant featuring a smooth gold frame with a glossy turquoise center that has subtle speckles, giving it a celestial appearance. A smaller gold star is embedded in the middle, enhancing its charm. The combination of gold and turquoise colors symbolizes elegance and tranquility, often associated with protection and positive energy in various cultures.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>star, gold-tone, turquoise, enamel, glitter, charm, jewelry, pendant</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปดาวที่มีกรอบสีทองเรียบเนียนและส่วนกลางสีฟ้าเทอร์ควอยซ์มันวาวที่มีจุดเล็กๆ ให้ความรู้สึกเหมือนท้องฟ้ายามค่ำคืน มีดาวเล็กสีทองฝังอยู่ตรงกลางเพิ่มความน่ารัก การผสมผสานของสีทองและฟ้าเทอร์ควอยซ์สื่อถึงความสง่างามและความสงบ ซึ่งในหลายวัฒนธรรมมักเชื่อมโยงกับการปกป้องและพลังบวก</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>star, pendant, gold, turquoise, jewelry, charm, elegant, celestial, glossy</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>ดาว, จี้, ทอง, ฟ้าเทอร์ควอยซ์, เครื่องประดับ, เสน่ห์, สง่างาม, ท้องฟ้า, มันวาว</t>
         </is>
       </c>
     </row>
@@ -1260,12 +1630,22 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>This elegant oval pendant features a polished gold frame encrusted with numerous small, sparkling white gemstones. The intricate pave setting creates a luxurious texture, making it a perfect accessory for adding a touch of sophistication and brilliance to any outfit.</t>
+          <t>This product is an elegant oval-shaped pendant featuring a polished gold frame. The interior surface is densely encrusted with numerous small, sparkling white stones, creating a luxurious and radiant effect. The combination of gold and white stones symbolizes wealth and purity, often associated with sophistication and timeless beauty in jewelry design.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>gold, oval, pendant, gemstones, pave, sparkling, luxury, jewelry</t>
+          <t>ผลิตภัณฑ์นี้เป็นจี้รูปไข่ที่มีกรอบทองเงางาม ภายในเต็มไปด้วยหินสีขาวเล็กๆ จำนวนมากที่ประดับอย่างแน่นหนา สร้างความหรูหราและเปล่งประกาย การผสมผสานระหว่างทองและหินสีขาวสื่อถึงความมั่งคั่งและความบริสุทธิ์ ซึ่งมักเกี่ยวข้องกับความสง่างามและความงามเหนือกาลเวลาในงานออกแบบเครื่องประดับ</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>pendant, oval, gold, white stones, luxury, jewelry, sparkling, elegant</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>จี้, รูปไข่, ทอง, หินสีขาว, หรูหรา, เครื่องประดับ, เปล่งประกาย, สง่างาม</t>
         </is>
       </c>
     </row>

</xml_diff>